<commit_message>
Add "Unit Cost" & "Total Cost" columns into ConsolidationAgingDataTable
</commit_message>
<xml_diff>
--- a/Report/3PL Report/3PL/JPN3PLReport.xlsx
+++ b/Report/3PL Report/3PL/JPN3PLReport.xlsx
@@ -755,7 +755,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,6 +765,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -807,6 +819,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,43 +1185,43 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>162</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="B2" s="4">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>73</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1215,43 +1229,43 @@
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>59</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>12</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1259,43 +1273,43 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1303,43 +1317,43 @@
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
-        <v>5100</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8046</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="B5" s="4">
+        <v>1500</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4755</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1347,87 +1361,87 @@
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
         <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2">
-        <v>1801</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2582</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="B7" s="4">
+        <v>2201</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1103</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1435,43 +1449,43 @@
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2">
-        <v>350</v>
-      </c>
-      <c r="C8" s="2">
-        <v>612</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="B8" s="4">
+        <v>885</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1479,43 +1493,43 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
         <v>1</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="4">
         <v>118</v>
       </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1523,43 +1537,43 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
         <v>1</v>
       </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
         <v>1</v>
       </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="N10" s="4">
         <v>500</v>
       </c>
     </row>
@@ -1567,43 +1581,43 @@
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
         <v>3</v>
       </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1611,43 +1625,43 @@
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>552</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0</v>
-      </c>
-      <c r="N12" s="2">
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>456</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1655,43 +1669,43 @@
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2">
-        <v>8008</v>
-      </c>
-      <c r="C13" s="2">
-        <v>10518</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2">
+      <c r="B13" s="4">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5">
+        <v>5308</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1699,43 +1713,43 @@
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2">
-        <v>10534</v>
-      </c>
-      <c r="C14" s="2">
-        <v>12369</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
+      <c r="B14" s="4">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5">
+        <v>12511</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1743,43 +1757,43 @@
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2">
-        <v>100</v>
-      </c>
-      <c r="C15" s="2">
-        <v>116</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2">
+      <c r="B15" s="4">
+        <v>115</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1787,43 +1801,43 @@
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>470</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0</v>
-      </c>
-      <c r="L16" s="2">
-        <v>0</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0</v>
-      </c>
-      <c r="N16" s="2">
+      <c r="B16" s="4">
+        <v>405</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>149</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1831,43 +1845,43 @@
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
         <v>3136</v>
       </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>801</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0</v>
-      </c>
-      <c r="N17" s="2">
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>746</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1875,43 +1889,43 @@
       <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="2">
-        <v>90</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2">
+      <c r="B18" s="4">
+        <v>50</v>
+      </c>
+      <c r="C18" s="5">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1919,43 +1933,43 @@
       <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0</v>
-      </c>
-      <c r="N19" s="2">
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1963,43 +1977,43 @@
       <c r="A20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="4">
         <v>300</v>
       </c>
-      <c r="C20" s="2">
-        <v>125</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2">
-        <v>0</v>
-      </c>
-      <c r="L20" s="2">
-        <v>0</v>
-      </c>
-      <c r="M20" s="2">
-        <v>0</v>
-      </c>
-      <c r="N20" s="2">
+      <c r="C20" s="5">
+        <v>263</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2007,43 +2021,43 @@
       <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="2">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
-        <v>0</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2">
-        <v>0</v>
-      </c>
-      <c r="L21" s="2">
-        <v>0</v>
-      </c>
-      <c r="M21" s="2">
-        <v>0</v>
-      </c>
-      <c r="N21" s="2">
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="5">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2051,43 +2065,43 @@
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="2">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2">
-        <v>0</v>
-      </c>
-      <c r="N22" s="2">
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2095,43 +2109,43 @@
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="2">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
         <v>1620</v>
       </c>
-      <c r="G23" s="2">
-        <v>915</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0</v>
-      </c>
-      <c r="N23" s="2">
+      <c r="H23" s="4">
+        <v>360</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2139,43 +2153,43 @@
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="2">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-      <c r="K24" s="2">
-        <v>0</v>
-      </c>
-      <c r="L24" s="2">
-        <v>0</v>
-      </c>
-      <c r="M24" s="2">
-        <v>0</v>
-      </c>
-      <c r="N24" s="2">
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0</v>
+      </c>
+      <c r="M24" s="5">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2183,43 +2197,43 @@
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="2">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0</v>
-      </c>
-      <c r="K25" s="2">
-        <v>0</v>
-      </c>
-      <c r="L25" s="2">
-        <v>0</v>
-      </c>
-      <c r="M25" s="2">
-        <v>0</v>
-      </c>
-      <c r="N25" s="2">
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0</v>
+      </c>
+      <c r="L25" s="4">
+        <v>0</v>
+      </c>
+      <c r="M25" s="5">
+        <v>0</v>
+      </c>
+      <c r="N25" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2227,43 +2241,43 @@
       <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="2">
-        <v>2000</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>664</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2">
-        <v>0</v>
-      </c>
-      <c r="M26" s="2">
-        <v>0</v>
-      </c>
-      <c r="N26" s="2">
+      <c r="B26" s="4">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5">
+        <v>717</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0</v>
+      </c>
+      <c r="M26" s="5">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2271,43 +2285,43 @@
       <c r="A27" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="2">
-        <v>8000</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1785</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0</v>
-      </c>
-      <c r="I27" s="2">
-        <v>0</v>
-      </c>
-      <c r="J27" s="2">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2">
-        <v>0</v>
-      </c>
-      <c r="M27" s="2">
-        <v>0</v>
-      </c>
-      <c r="N27" s="2">
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>7682</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0</v>
+      </c>
+      <c r="M27" s="5">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2315,43 +2329,43 @@
       <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="2">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <v>0</v>
-      </c>
-      <c r="J28" s="2">
-        <v>0</v>
-      </c>
-      <c r="K28" s="2">
-        <v>0</v>
-      </c>
-      <c r="L28" s="2">
-        <v>0</v>
-      </c>
-      <c r="M28" s="2">
-        <v>0</v>
-      </c>
-      <c r="N28" s="2">
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
+        <v>0</v>
+      </c>
+      <c r="M28" s="5">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2359,43 +2373,43 @@
       <c r="A29" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="2">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2">
-        <v>8440</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0</v>
-      </c>
-      <c r="I29" s="2">
-        <v>0</v>
-      </c>
-      <c r="J29" s="2">
-        <v>0</v>
-      </c>
-      <c r="K29" s="2">
-        <v>0</v>
-      </c>
-      <c r="L29" s="2">
-        <v>0</v>
-      </c>
-      <c r="M29" s="2">
-        <v>0</v>
-      </c>
-      <c r="N29" s="2">
+      <c r="B29" s="4">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>7659</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0</v>
+      </c>
+      <c r="K29" s="5">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>0</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+      <c r="N29" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2403,43 +2417,43 @@
       <c r="A30" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="2">
-        <v>1196</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
-      <c r="I30" s="2">
-        <v>0</v>
-      </c>
-      <c r="J30" s="2">
-        <v>0</v>
-      </c>
-      <c r="K30" s="2">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0</v>
-      </c>
-      <c r="M30" s="2">
-        <v>0</v>
-      </c>
-      <c r="N30" s="2">
+      <c r="B30" s="4">
+        <v>272</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+      <c r="K30" s="5">
+        <v>0</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0</v>
+      </c>
+      <c r="M30" s="5">
+        <v>0</v>
+      </c>
+      <c r="N30" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2447,41 +2461,43 @@
       <c r="A31" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="2">
-        <v>2000</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1141</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0</v>
-      </c>
-      <c r="I31" s="2">
-        <v>0</v>
-      </c>
-      <c r="J31" s="2">
-        <v>0</v>
-      </c>
-      <c r="K31" s="2">
-        <v>0</v>
-      </c>
-      <c r="L31" s="2">
-        <v>0</v>
-      </c>
-      <c r="M31" s="2">
-        <v>0</v>
-      </c>
-      <c r="N31" s="2">
+      <c r="B31" s="4">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1776</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0</v>
+      </c>
+      <c r="M31" s="5">
+        <v>0</v>
+      </c>
+      <c r="N31" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2489,43 +2505,43 @@
       <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5">
         <v>1500</v>
       </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
         <v>1600</v>
       </c>
-      <c r="E32" s="2">
+      <c r="F32" s="4">
         <v>400</v>
       </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-      <c r="I32" s="2">
-        <v>0</v>
-      </c>
-      <c r="J32" s="2">
-        <v>0</v>
-      </c>
-      <c r="K32" s="2">
-        <v>0</v>
-      </c>
-      <c r="L32" s="2">
-        <v>0</v>
-      </c>
-      <c r="M32" s="2">
-        <v>0</v>
-      </c>
-      <c r="N32" s="2">
+      <c r="G32" s="5">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0</v>
+      </c>
+      <c r="K32" s="5">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4">
+        <v>0</v>
+      </c>
+      <c r="M32" s="5">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add "Unit Cost" & "Total Cost" data into Consolidation AgingData Table.
</commit_message>
<xml_diff>
--- a/Report/3PL Report/3PL/JPN3PLReport.xlsx
+++ b/Report/3PL Report/3PL/JPN3PLReport.xlsx
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="5">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
@@ -1318,10 +1318,10 @@
         <v>16</v>
       </c>
       <c r="B5" s="4">
-        <v>1500</v>
+        <v>1502</v>
       </c>
       <c r="C5" s="5">
-        <v>4755</v>
+        <v>2693</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -1406,10 +1406,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="4">
-        <v>2201</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5">
-        <v>1103</v>
+        <v>0</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -1450,7 +1450,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="4">
-        <v>885</v>
+        <v>712</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -1521,10 +1521,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M9" s="5">
         <v>0</v>
@@ -1565,10 +1565,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
         <v>1</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
       </c>
       <c r="M10" s="5">
         <v>1</v>
@@ -1632,10 +1632,10 @@
         <v>0</v>
       </c>
       <c r="D12" s="4">
-        <v>456</v>
+        <v>0</v>
       </c>
       <c r="E12" s="5">
-        <v>0</v>
+        <v>435</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -1670,10 +1670,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="4">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="5">
-        <v>5308</v>
+        <v>1882</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -1714,10 +1714,10 @@
         <v>25</v>
       </c>
       <c r="B14" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="5">
-        <v>12511</v>
+        <v>5685</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -1758,7 +1758,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="4">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="C15" s="5">
         <v>0</v>
@@ -1808,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="4">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -1849,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="5">
-        <v>0</v>
+        <v>3136</v>
       </c>
       <c r="D17" s="4">
-        <v>3136</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -1893,7 +1893,7 @@
         <v>50</v>
       </c>
       <c r="C18" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D18" s="4">
         <v>0</v>
@@ -1978,10 +1978,10 @@
         <v>31</v>
       </c>
       <c r="B20" s="4">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C20" s="5">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -2245,7 +2245,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="5">
-        <v>717</v>
+        <v>188</v>
       </c>
       <c r="D26" s="4">
         <v>0</v>
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="5">
-        <v>7682</v>
+        <v>7067</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
@@ -2392,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="4">
-        <v>7659</v>
+        <v>7577</v>
       </c>
       <c r="I29" s="5">
         <v>0</v>
@@ -2418,7 +2418,7 @@
         <v>41</v>
       </c>
       <c r="B30" s="4">
-        <v>272</v>
+        <v>1201</v>
       </c>
       <c r="C30" s="5">
         <v>0</v>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="5">
-        <v>1776</v>
+        <v>1441</v>
       </c>
       <c r="D31" s="4">
         <v>0</v>

</xml_diff>